<commit_message>
trying out different options
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\github\data-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\data-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="280">
   <si>
     <t>Column1</t>
   </si>
@@ -854,9 +854,6 @@
     <t>Program
 Specific
 Comment</t>
-  </si>
-  <si>
-    <t>LEA Comment</t>
   </si>
   <si>
     <t>COMMENT</t>
@@ -3365,7 +3362,7 @@
   <dimension ref="A1:BJ172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3798,7 +3795,9 @@
       <c r="A3" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="23">
+        <v>1</v>
+      </c>
       <c r="C3" s="24"/>
       <c r="D3" s="25" t="s">
         <v>61</v>
@@ -3979,10 +3978,10 @@
         <v>274</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>275</v>
@@ -4163,14 +4162,16 @@
       <c r="B5" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>276</v>
+      <c r="C5" s="3">
+        <v>1</v>
       </c>
       <c r="D5" s="3">
-        <v>100</v>
+        <f>B3+10</f>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
-        <v>20000</v>
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>12</v>
       </c>
       <c r="F5" s="3">
         <v>30</v>
@@ -4343,13 +4344,17 @@
       <c r="B6" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>276</v>
+      <c r="C6" s="3">
+        <v>1</v>
       </c>
       <c r="D6" s="3">
-        <v>100</v>
-      </c>
-      <c r="E6" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -4413,13 +4418,17 @@
       <c r="B7" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>276</v>
+      <c r="C7" s="3">
+        <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>100</v>
-      </c>
-      <c r="E7" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -4483,13 +4492,17 @@
       <c r="B8" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>276</v>
+      <c r="C8" s="3">
+        <v>3</v>
       </c>
       <c r="D8" s="3">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>6</v>
+      </c>
+      <c r="E8" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>9</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -4553,13 +4566,17 @@
       <c r="B9" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>276</v>
+      <c r="C9" s="3">
+        <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>100</v>
-      </c>
-      <c r="E9" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -4623,13 +4640,17 @@
       <c r="B10" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>276</v>
+      <c r="C10" s="3">
+        <v>1</v>
       </c>
       <c r="D10" s="3">
-        <v>100</v>
-      </c>
-      <c r="E10" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E10" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -4693,13 +4714,17 @@
       <c r="B11" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>276</v>
+      <c r="C11" s="3">
+        <v>1</v>
       </c>
       <c r="D11" s="3">
-        <v>100</v>
-      </c>
-      <c r="E11" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -4763,13 +4788,17 @@
       <c r="B12" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>276</v>
+      <c r="C12" s="3">
+        <v>1</v>
       </c>
       <c r="D12" s="3">
-        <v>100</v>
-      </c>
-      <c r="E12" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -4833,13 +4862,17 @@
       <c r="B13" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>276</v>
+      <c r="C13" s="3">
+        <v>1</v>
       </c>
       <c r="D13" s="3">
-        <v>100</v>
-      </c>
-      <c r="E13" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -4903,13 +4936,17 @@
       <c r="B14" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>276</v>
+      <c r="C14" s="3">
+        <v>1</v>
       </c>
       <c r="D14" s="3">
-        <v>100</v>
-      </c>
-      <c r="E14" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -4973,13 +5010,17 @@
       <c r="B15" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>276</v>
+      <c r="C15" s="3">
+        <v>1</v>
       </c>
       <c r="D15" s="3">
-        <v>100</v>
-      </c>
-      <c r="E15" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -5043,13 +5084,17 @@
       <c r="B16" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>276</v>
+      <c r="C16" s="3">
+        <v>1</v>
       </c>
       <c r="D16" s="3">
-        <v>100</v>
-      </c>
-      <c r="E16" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E16" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -5113,13 +5158,17 @@
       <c r="B17" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>276</v>
+      <c r="C17" s="3">
+        <v>1</v>
       </c>
       <c r="D17" s="3">
-        <v>100</v>
-      </c>
-      <c r="E17" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E17" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -5183,13 +5232,17 @@
       <c r="B18" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>276</v>
+      <c r="C18" s="3">
+        <v>1</v>
       </c>
       <c r="D18" s="3">
-        <v>100</v>
-      </c>
-      <c r="E18" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E18" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -5253,13 +5306,17 @@
       <c r="B19" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>276</v>
+      <c r="C19" s="3">
+        <v>1</v>
       </c>
       <c r="D19" s="3">
-        <v>100</v>
-      </c>
-      <c r="E19" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E19" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -5323,13 +5380,17 @@
       <c r="B20" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>276</v>
+      <c r="C20" s="3">
+        <v>1</v>
       </c>
       <c r="D20" s="3">
-        <v>100</v>
-      </c>
-      <c r="E20" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E20" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -5393,13 +5454,17 @@
       <c r="B21" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>276</v>
+      <c r="C21" s="3">
+        <v>1</v>
       </c>
       <c r="D21" s="3">
-        <v>100</v>
-      </c>
-      <c r="E21" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -5463,13 +5528,17 @@
       <c r="B22" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>276</v>
+      <c r="C22" s="3">
+        <v>1</v>
       </c>
       <c r="D22" s="3">
-        <v>100</v>
-      </c>
-      <c r="E22" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E22" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -5533,13 +5602,17 @@
       <c r="B23" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>276</v>
+      <c r="C23" s="3">
+        <v>1</v>
       </c>
       <c r="D23" s="3">
-        <v>100</v>
-      </c>
-      <c r="E23" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E23" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -5603,13 +5676,17 @@
       <c r="B24" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>276</v>
+      <c r="C24" s="3">
+        <v>1</v>
       </c>
       <c r="D24" s="3">
-        <v>100</v>
-      </c>
-      <c r="E24" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E24" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -5673,13 +5750,17 @@
       <c r="B25" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>276</v>
+      <c r="C25" s="3">
+        <v>1</v>
       </c>
       <c r="D25" s="3">
-        <v>100</v>
-      </c>
-      <c r="E25" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E25" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -5743,13 +5824,17 @@
       <c r="B26" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>276</v>
+      <c r="C26" s="3">
+        <v>1</v>
       </c>
       <c r="D26" s="3">
-        <v>100</v>
-      </c>
-      <c r="E26" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E26" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -5813,13 +5898,17 @@
       <c r="B27" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>276</v>
+      <c r="C27" s="3">
+        <v>1</v>
       </c>
       <c r="D27" s="3">
-        <v>100</v>
-      </c>
-      <c r="E27" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E27" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -5883,13 +5972,17 @@
       <c r="B28" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>276</v>
+      <c r="C28" s="3">
+        <v>1</v>
       </c>
       <c r="D28" s="3">
-        <v>100</v>
-      </c>
-      <c r="E28" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E28" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -5953,13 +6046,17 @@
       <c r="B29" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>276</v>
+      <c r="C29" s="3">
+        <v>1</v>
       </c>
       <c r="D29" s="3">
-        <v>100</v>
-      </c>
-      <c r="E29" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E29" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -6023,13 +6120,17 @@
       <c r="B30" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>276</v>
+      <c r="C30" s="3">
+        <v>1</v>
       </c>
       <c r="D30" s="3">
-        <v>100</v>
-      </c>
-      <c r="E30" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E30" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -6093,13 +6194,17 @@
       <c r="B31" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>276</v>
+      <c r="C31" s="3">
+        <v>1</v>
       </c>
       <c r="D31" s="3">
-        <v>100</v>
-      </c>
-      <c r="E31" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E31" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -6163,13 +6268,17 @@
       <c r="B32" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>276</v>
+      <c r="C32" s="3">
+        <v>1</v>
       </c>
       <c r="D32" s="3">
-        <v>100</v>
-      </c>
-      <c r="E32" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E32" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -6233,13 +6342,17 @@
       <c r="B33" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>276</v>
+      <c r="C33" s="3">
+        <v>1</v>
       </c>
       <c r="D33" s="3">
-        <v>100</v>
-      </c>
-      <c r="E33" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E33" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -6303,13 +6416,17 @@
       <c r="B34" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>276</v>
+      <c r="C34" s="3">
+        <v>1</v>
       </c>
       <c r="D34" s="3">
-        <v>100</v>
-      </c>
-      <c r="E34" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E34" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -6373,13 +6490,17 @@
       <c r="B35" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>276</v>
+      <c r="C35" s="3">
+        <v>1</v>
       </c>
       <c r="D35" s="3">
-        <v>100</v>
-      </c>
-      <c r="E35" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E35" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -6443,13 +6564,17 @@
       <c r="B36" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>276</v>
+      <c r="C36" s="3">
+        <v>1</v>
       </c>
       <c r="D36" s="3">
-        <v>100</v>
-      </c>
-      <c r="E36" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E36" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -6513,13 +6638,17 @@
       <c r="B37" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>276</v>
+      <c r="C37" s="3">
+        <v>1</v>
       </c>
       <c r="D37" s="3">
-        <v>100</v>
-      </c>
-      <c r="E37" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E37" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -6583,13 +6712,17 @@
       <c r="B38" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>276</v>
+      <c r="C38" s="3">
+        <v>1</v>
       </c>
       <c r="D38" s="3">
-        <v>100</v>
-      </c>
-      <c r="E38" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E38" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -6653,13 +6786,17 @@
       <c r="B39" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>276</v>
+      <c r="C39" s="3">
+        <v>1</v>
       </c>
       <c r="D39" s="3">
-        <v>100</v>
-      </c>
-      <c r="E39" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E39" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -6723,13 +6860,17 @@
       <c r="B40" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>276</v>
+      <c r="C40" s="3">
+        <v>1</v>
       </c>
       <c r="D40" s="3">
-        <v>100</v>
-      </c>
-      <c r="E40" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E40" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -6793,13 +6934,17 @@
       <c r="B41" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>276</v>
+      <c r="C41" s="3">
+        <v>1</v>
       </c>
       <c r="D41" s="3">
-        <v>100</v>
-      </c>
-      <c r="E41" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E41" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -6863,13 +7008,17 @@
       <c r="B42" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>276</v>
+      <c r="C42" s="3">
+        <v>1</v>
       </c>
       <c r="D42" s="3">
-        <v>100</v>
-      </c>
-      <c r="E42" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E42" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -6933,13 +7082,17 @@
       <c r="B43" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>276</v>
+      <c r="C43" s="3">
+        <v>1</v>
       </c>
       <c r="D43" s="3">
-        <v>100</v>
-      </c>
-      <c r="E43" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E43" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -7003,13 +7156,17 @@
       <c r="B44" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>276</v>
+      <c r="C44" s="3">
+        <v>1</v>
       </c>
       <c r="D44" s="3">
-        <v>100</v>
-      </c>
-      <c r="E44" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E44" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -7073,13 +7230,17 @@
       <c r="B45" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>276</v>
+      <c r="C45" s="3">
+        <v>1</v>
       </c>
       <c r="D45" s="3">
-        <v>100</v>
-      </c>
-      <c r="E45" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E45" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -7143,13 +7304,17 @@
       <c r="B46" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>276</v>
+      <c r="C46" s="3">
+        <v>1</v>
       </c>
       <c r="D46" s="3">
-        <v>100</v>
-      </c>
-      <c r="E46" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E46" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -7213,13 +7378,17 @@
       <c r="B47" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>276</v>
+      <c r="C47" s="3">
+        <v>1</v>
       </c>
       <c r="D47" s="3">
-        <v>100</v>
-      </c>
-      <c r="E47" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E47" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -7283,13 +7452,17 @@
       <c r="B48" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>276</v>
+      <c r="C48" s="3">
+        <v>1</v>
       </c>
       <c r="D48" s="3">
-        <v>100</v>
-      </c>
-      <c r="E48" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E48" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -7353,13 +7526,17 @@
       <c r="B49" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>276</v>
+      <c r="C49" s="3">
+        <v>1</v>
       </c>
       <c r="D49" s="3">
-        <v>100</v>
-      </c>
-      <c r="E49" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E49" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -7423,13 +7600,17 @@
       <c r="B50" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>276</v>
+      <c r="C50" s="3">
+        <v>1</v>
       </c>
       <c r="D50" s="3">
-        <v>100</v>
-      </c>
-      <c r="E50" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E50" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -7493,13 +7674,17 @@
       <c r="B51" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>276</v>
+      <c r="C51" s="3">
+        <v>1</v>
       </c>
       <c r="D51" s="3">
-        <v>100</v>
-      </c>
-      <c r="E51" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E51" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -7563,13 +7748,17 @@
       <c r="B52" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>276</v>
+      <c r="C52" s="3">
+        <v>1</v>
       </c>
       <c r="D52" s="3">
-        <v>100</v>
-      </c>
-      <c r="E52" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E52" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -7633,13 +7822,17 @@
       <c r="B53" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>276</v>
+      <c r="C53" s="3">
+        <v>1</v>
       </c>
       <c r="D53" s="3">
-        <v>100</v>
-      </c>
-      <c r="E53" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E53" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
@@ -7703,13 +7896,17 @@
       <c r="B54" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>276</v>
+      <c r="C54" s="3">
+        <v>1</v>
       </c>
       <c r="D54" s="3">
-        <v>100</v>
-      </c>
-      <c r="E54" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E54" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -7773,13 +7970,17 @@
       <c r="B55" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>276</v>
+      <c r="C55" s="3">
+        <v>1</v>
       </c>
       <c r="D55" s="3">
-        <v>100</v>
-      </c>
-      <c r="E55" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E55" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
@@ -7843,13 +8044,17 @@
       <c r="B56" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>276</v>
+      <c r="C56" s="3">
+        <v>1</v>
       </c>
       <c r="D56" s="3">
-        <v>100</v>
-      </c>
-      <c r="E56" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E56" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
@@ -7913,13 +8118,17 @@
       <c r="B57" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>276</v>
+      <c r="C57" s="3">
+        <v>1</v>
       </c>
       <c r="D57" s="3">
-        <v>100</v>
-      </c>
-      <c r="E57" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E57" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -7983,13 +8192,17 @@
       <c r="B58" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>276</v>
+      <c r="C58" s="3">
+        <v>1</v>
       </c>
       <c r="D58" s="3">
-        <v>100</v>
-      </c>
-      <c r="E58" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E58" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -8053,13 +8266,17 @@
       <c r="B59" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>276</v>
+      <c r="C59" s="3">
+        <v>1</v>
       </c>
       <c r="D59" s="3">
-        <v>100</v>
-      </c>
-      <c r="E59" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E59" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
@@ -8123,13 +8340,17 @@
       <c r="B60" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>276</v>
+      <c r="C60" s="3">
+        <v>1</v>
       </c>
       <c r="D60" s="3">
-        <v>100</v>
-      </c>
-      <c r="E60" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E60" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -8193,13 +8414,17 @@
       <c r="B61" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>276</v>
+      <c r="C61" s="3">
+        <v>1</v>
       </c>
       <c r="D61" s="3">
-        <v>100</v>
-      </c>
-      <c r="E61" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E61" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
@@ -8263,13 +8488,17 @@
       <c r="B62" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>276</v>
+      <c r="C62" s="3">
+        <v>1</v>
       </c>
       <c r="D62" s="3">
-        <v>100</v>
-      </c>
-      <c r="E62" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E62" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -8333,13 +8562,17 @@
       <c r="B63" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>276</v>
+      <c r="C63" s="3">
+        <v>1</v>
       </c>
       <c r="D63" s="3">
-        <v>100</v>
-      </c>
-      <c r="E63" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E63" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
@@ -8403,13 +8636,17 @@
       <c r="B64" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>276</v>
+      <c r="C64" s="3">
+        <v>1</v>
       </c>
       <c r="D64" s="3">
-        <v>100</v>
-      </c>
-      <c r="E64" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E64" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
@@ -8473,13 +8710,17 @@
       <c r="B65" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>276</v>
+      <c r="C65" s="3">
+        <v>1</v>
       </c>
       <c r="D65" s="3">
-        <v>100</v>
-      </c>
-      <c r="E65" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E65" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
@@ -8543,13 +8784,17 @@
       <c r="B66" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>276</v>
+      <c r="C66" s="3">
+        <v>1</v>
       </c>
       <c r="D66" s="3">
-        <v>100</v>
-      </c>
-      <c r="E66" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E66" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -8613,13 +8858,17 @@
       <c r="B67" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>276</v>
+      <c r="C67" s="3">
+        <v>1</v>
       </c>
       <c r="D67" s="3">
-        <v>100</v>
-      </c>
-      <c r="E67" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E67" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
@@ -8683,13 +8932,17 @@
       <c r="B68" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>276</v>
+      <c r="C68" s="3">
+        <v>1</v>
       </c>
       <c r="D68" s="3">
-        <v>100</v>
-      </c>
-      <c r="E68" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E68" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
@@ -8753,13 +9006,17 @@
       <c r="B69" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>276</v>
+      <c r="C69" s="3">
+        <v>1</v>
       </c>
       <c r="D69" s="3">
-        <v>100</v>
-      </c>
-      <c r="E69" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E69" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
@@ -8823,13 +9080,17 @@
       <c r="B70" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>276</v>
+      <c r="C70" s="3">
+        <v>1</v>
       </c>
       <c r="D70" s="3">
-        <v>100</v>
-      </c>
-      <c r="E70" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E70" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
@@ -8893,13 +9154,17 @@
       <c r="B71" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>276</v>
+      <c r="C71" s="3">
+        <v>1</v>
       </c>
       <c r="D71" s="3">
-        <v>100</v>
-      </c>
-      <c r="E71" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E71" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
@@ -8963,13 +9228,17 @@
       <c r="B72" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>276</v>
+      <c r="C72" s="3">
+        <v>1</v>
       </c>
       <c r="D72" s="3">
-        <v>100</v>
-      </c>
-      <c r="E72" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E72" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
@@ -9033,13 +9302,17 @@
       <c r="B73" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>276</v>
+      <c r="C73" s="3">
+        <v>1</v>
       </c>
       <c r="D73" s="3">
-        <v>100</v>
-      </c>
-      <c r="E73" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E73" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
@@ -9103,13 +9376,17 @@
       <c r="B74" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>276</v>
+      <c r="C74" s="3">
+        <v>1</v>
       </c>
       <c r="D74" s="3">
-        <v>100</v>
-      </c>
-      <c r="E74" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E74" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
@@ -9173,13 +9450,17 @@
       <c r="B75" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>276</v>
+      <c r="C75" s="3">
+        <v>1</v>
       </c>
       <c r="D75" s="3">
-        <v>100</v>
-      </c>
-      <c r="E75" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E75" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
@@ -9243,13 +9524,17 @@
       <c r="B76" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>276</v>
+      <c r="C76" s="3">
+        <v>1</v>
       </c>
       <c r="D76" s="3">
-        <v>100</v>
-      </c>
-      <c r="E76" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E76" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
@@ -9313,13 +9598,17 @@
       <c r="B77" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C77" s="3" t="s">
-        <v>276</v>
+      <c r="C77" s="3">
+        <v>1</v>
       </c>
       <c r="D77" s="3">
-        <v>100</v>
-      </c>
-      <c r="E77" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E77" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
@@ -9383,13 +9672,17 @@
       <c r="B78" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C78" s="3" t="s">
-        <v>276</v>
+      <c r="C78" s="3">
+        <v>1</v>
       </c>
       <c r="D78" s="3">
-        <v>100</v>
-      </c>
-      <c r="E78" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E78" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
@@ -9453,13 +9746,17 @@
       <c r="B79" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C79" s="3" t="s">
-        <v>276</v>
+      <c r="C79" s="3">
+        <v>1</v>
       </c>
       <c r="D79" s="3">
-        <v>100</v>
-      </c>
-      <c r="E79" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E79" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
@@ -9523,13 +9820,17 @@
       <c r="B80" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="C80" s="3" t="s">
-        <v>276</v>
+      <c r="C80" s="3">
+        <v>1</v>
       </c>
       <c r="D80" s="3">
-        <v>100</v>
-      </c>
-      <c r="E80" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E80" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
@@ -9593,13 +9894,17 @@
       <c r="B81" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C81" s="3" t="s">
-        <v>276</v>
+      <c r="C81" s="3">
+        <v>1</v>
       </c>
       <c r="D81" s="3">
-        <v>100</v>
-      </c>
-      <c r="E81" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E81" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
@@ -9663,13 +9968,17 @@
       <c r="B82" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>276</v>
+      <c r="C82" s="3">
+        <v>1</v>
       </c>
       <c r="D82" s="3">
-        <v>100</v>
-      </c>
-      <c r="E82" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E82" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
@@ -9733,13 +10042,17 @@
       <c r="B83" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>276</v>
+      <c r="C83" s="3">
+        <v>1</v>
       </c>
       <c r="D83" s="3">
-        <v>100</v>
-      </c>
-      <c r="E83" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E83" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
@@ -9803,13 +10116,17 @@
       <c r="B84" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C84" s="3" t="s">
-        <v>276</v>
+      <c r="C84" s="3">
+        <v>1</v>
       </c>
       <c r="D84" s="3">
-        <v>100</v>
-      </c>
-      <c r="E84" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E84" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
@@ -9873,13 +10190,17 @@
       <c r="B85" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>276</v>
+      <c r="C85" s="3">
+        <v>1</v>
       </c>
       <c r="D85" s="3">
-        <v>100</v>
-      </c>
-      <c r="E85" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E85" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
@@ -9943,13 +10264,17 @@
       <c r="B86" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>276</v>
+      <c r="C86" s="3">
+        <v>1</v>
       </c>
       <c r="D86" s="3">
-        <v>100</v>
-      </c>
-      <c r="E86" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E86" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
@@ -10013,13 +10338,17 @@
       <c r="B87" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C87" s="3" t="s">
-        <v>276</v>
+      <c r="C87" s="3">
+        <v>1</v>
       </c>
       <c r="D87" s="3">
-        <v>100</v>
-      </c>
-      <c r="E87" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E87" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
@@ -10083,13 +10412,17 @@
       <c r="B88" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>276</v>
+      <c r="C88" s="3">
+        <v>1</v>
       </c>
       <c r="D88" s="3">
-        <v>100</v>
-      </c>
-      <c r="E88" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E88" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
@@ -10153,13 +10486,17 @@
       <c r="B89" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>276</v>
+      <c r="C89" s="3">
+        <v>1</v>
       </c>
       <c r="D89" s="3">
-        <v>100</v>
-      </c>
-      <c r="E89" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E89" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
@@ -10223,13 +10560,17 @@
       <c r="B90" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>276</v>
+      <c r="C90" s="3">
+        <v>1</v>
       </c>
       <c r="D90" s="3">
-        <v>100</v>
-      </c>
-      <c r="E90" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E90" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
@@ -10293,13 +10634,17 @@
       <c r="B91" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>276</v>
+      <c r="C91" s="3">
+        <v>1</v>
       </c>
       <c r="D91" s="3">
-        <v>100</v>
-      </c>
-      <c r="E91" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E91" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
@@ -10363,13 +10708,17 @@
       <c r="B92" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="C92" s="3" t="s">
-        <v>276</v>
+      <c r="C92" s="3">
+        <v>1</v>
       </c>
       <c r="D92" s="3">
-        <v>100</v>
-      </c>
-      <c r="E92" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E92" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
@@ -10433,13 +10782,17 @@
       <c r="B93" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>276</v>
+      <c r="C93" s="3">
+        <v>1</v>
       </c>
       <c r="D93" s="3">
-        <v>100</v>
-      </c>
-      <c r="E93" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E93" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
@@ -10503,13 +10856,17 @@
       <c r="B94" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="C94" s="3" t="s">
-        <v>276</v>
+      <c r="C94" s="3">
+        <v>1</v>
       </c>
       <c r="D94" s="3">
-        <v>100</v>
-      </c>
-      <c r="E94" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E94" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
@@ -10573,13 +10930,17 @@
       <c r="B95" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>276</v>
+      <c r="C95" s="3">
+        <v>1</v>
       </c>
       <c r="D95" s="3">
-        <v>100</v>
-      </c>
-      <c r="E95" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E95" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
@@ -10643,13 +11004,17 @@
       <c r="B96" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>276</v>
+      <c r="C96" s="3">
+        <v>1</v>
       </c>
       <c r="D96" s="3">
-        <v>100</v>
-      </c>
-      <c r="E96" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E96" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
@@ -10713,13 +11078,17 @@
       <c r="B97" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C97" s="3" t="s">
-        <v>276</v>
+      <c r="C97" s="3">
+        <v>1</v>
       </c>
       <c r="D97" s="3">
-        <v>100</v>
-      </c>
-      <c r="E97" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E97" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
@@ -10783,13 +11152,17 @@
       <c r="B98" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C98" s="3" t="s">
-        <v>276</v>
+      <c r="C98" s="3">
+        <v>1</v>
       </c>
       <c r="D98" s="3">
-        <v>100</v>
-      </c>
-      <c r="E98" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E98" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
@@ -10853,13 +11226,17 @@
       <c r="B99" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>276</v>
+      <c r="C99" s="3">
+        <v>1</v>
       </c>
       <c r="D99" s="3">
-        <v>100</v>
-      </c>
-      <c r="E99" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E99" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
@@ -10923,13 +11300,17 @@
       <c r="B100" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>276</v>
+      <c r="C100" s="3">
+        <v>1</v>
       </c>
       <c r="D100" s="3">
-        <v>100</v>
-      </c>
-      <c r="E100" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E100" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
@@ -10993,13 +11374,17 @@
       <c r="B101" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>276</v>
+      <c r="C101" s="3">
+        <v>1</v>
       </c>
       <c r="D101" s="3">
-        <v>100</v>
-      </c>
-      <c r="E101" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E101" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
@@ -11063,13 +11448,17 @@
       <c r="B102" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>276</v>
+      <c r="C102" s="3">
+        <v>1</v>
       </c>
       <c r="D102" s="3">
-        <v>100</v>
-      </c>
-      <c r="E102" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E102" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
@@ -11133,13 +11522,17 @@
       <c r="B103" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C103" s="3" t="s">
-        <v>276</v>
+      <c r="C103" s="3">
+        <v>1</v>
       </c>
       <c r="D103" s="3">
-        <v>100</v>
-      </c>
-      <c r="E103" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E103" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
@@ -11203,13 +11596,17 @@
       <c r="B104" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C104" s="3" t="s">
-        <v>276</v>
+      <c r="C104" s="3">
+        <v>1</v>
       </c>
       <c r="D104" s="3">
-        <v>100</v>
-      </c>
-      <c r="E104" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E104" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
@@ -11273,13 +11670,17 @@
       <c r="B105" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C105" s="3" t="s">
-        <v>276</v>
+      <c r="C105" s="3">
+        <v>1</v>
       </c>
       <c r="D105" s="3">
-        <v>100</v>
-      </c>
-      <c r="E105" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E105" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
@@ -11343,13 +11744,17 @@
       <c r="B106" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C106" s="3" t="s">
-        <v>276</v>
+      <c r="C106" s="3">
+        <v>1</v>
       </c>
       <c r="D106" s="3">
-        <v>100</v>
-      </c>
-      <c r="E106" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E106" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
@@ -11413,13 +11818,17 @@
       <c r="B107" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>276</v>
+      <c r="C107" s="3">
+        <v>1</v>
       </c>
       <c r="D107" s="3">
-        <v>100</v>
-      </c>
-      <c r="E107" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E107" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
@@ -11483,13 +11892,17 @@
       <c r="B108" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>276</v>
+      <c r="C108" s="3">
+        <v>1</v>
       </c>
       <c r="D108" s="3">
-        <v>100</v>
-      </c>
-      <c r="E108" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E108" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F108" s="3"/>
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
@@ -11553,13 +11966,17 @@
       <c r="B109" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C109" s="3" t="s">
-        <v>276</v>
+      <c r="C109" s="3">
+        <v>1</v>
       </c>
       <c r="D109" s="3">
-        <v>100</v>
-      </c>
-      <c r="E109" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E109" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
@@ -11623,13 +12040,17 @@
       <c r="B110" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C110" s="3" t="s">
-        <v>276</v>
+      <c r="C110" s="3">
+        <v>1</v>
       </c>
       <c r="D110" s="3">
-        <v>100</v>
-      </c>
-      <c r="E110" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E110" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
@@ -11693,13 +12114,17 @@
       <c r="B111" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C111" s="3" t="s">
-        <v>276</v>
+      <c r="C111" s="3">
+        <v>1</v>
       </c>
       <c r="D111" s="3">
-        <v>100</v>
-      </c>
-      <c r="E111" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E111" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
@@ -11763,13 +12188,17 @@
       <c r="B112" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>276</v>
+      <c r="C112" s="3">
+        <v>1</v>
       </c>
       <c r="D112" s="3">
-        <v>100</v>
-      </c>
-      <c r="E112" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E112" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
@@ -11833,13 +12262,17 @@
       <c r="B113" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="C113" s="3" t="s">
-        <v>276</v>
+      <c r="C113" s="3">
+        <v>1</v>
       </c>
       <c r="D113" s="3">
-        <v>100</v>
-      </c>
-      <c r="E113" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E113" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
@@ -11903,13 +12336,17 @@
       <c r="B114" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="C114" s="3" t="s">
-        <v>276</v>
+      <c r="C114" s="3">
+        <v>1</v>
       </c>
       <c r="D114" s="3">
-        <v>100</v>
-      </c>
-      <c r="E114" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E114" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
@@ -11973,13 +12410,17 @@
       <c r="B115" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C115" s="3" t="s">
-        <v>276</v>
+      <c r="C115" s="3">
+        <v>1</v>
       </c>
       <c r="D115" s="3">
-        <v>100</v>
-      </c>
-      <c r="E115" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E115" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F115" s="3"/>
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
@@ -12043,13 +12484,17 @@
       <c r="B116" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C116" s="3" t="s">
-        <v>276</v>
+      <c r="C116" s="3">
+        <v>1</v>
       </c>
       <c r="D116" s="3">
-        <v>100</v>
-      </c>
-      <c r="E116" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E116" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
@@ -12113,13 +12558,17 @@
       <c r="B117" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C117" s="3" t="s">
-        <v>276</v>
+      <c r="C117" s="3">
+        <v>1</v>
       </c>
       <c r="D117" s="3">
-        <v>100</v>
-      </c>
-      <c r="E117" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E117" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
@@ -12183,13 +12632,17 @@
       <c r="B118" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="C118" s="3" t="s">
-        <v>276</v>
+      <c r="C118" s="3">
+        <v>1</v>
       </c>
       <c r="D118" s="3">
-        <v>100</v>
-      </c>
-      <c r="E118" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E118" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
@@ -12253,13 +12706,17 @@
       <c r="B119" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="C119" s="3" t="s">
-        <v>276</v>
+      <c r="C119" s="3">
+        <v>1</v>
       </c>
       <c r="D119" s="3">
-        <v>100</v>
-      </c>
-      <c r="E119" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E119" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
@@ -12323,13 +12780,17 @@
       <c r="B120" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>276</v>
+      <c r="C120" s="3">
+        <v>1</v>
       </c>
       <c r="D120" s="3">
-        <v>100</v>
-      </c>
-      <c r="E120" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E120" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
@@ -12393,13 +12854,17 @@
       <c r="B121" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C121" s="3" t="s">
-        <v>276</v>
+      <c r="C121" s="3">
+        <v>1</v>
       </c>
       <c r="D121" s="3">
-        <v>100</v>
-      </c>
-      <c r="E121" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E121" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
@@ -12463,13 +12928,17 @@
       <c r="B122" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C122" s="3" t="s">
-        <v>276</v>
+      <c r="C122" s="3">
+        <v>1</v>
       </c>
       <c r="D122" s="3">
-        <v>100</v>
-      </c>
-      <c r="E122" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E122" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
@@ -12533,13 +13002,17 @@
       <c r="B123" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="C123" s="3" t="s">
-        <v>276</v>
+      <c r="C123" s="3">
+        <v>1</v>
       </c>
       <c r="D123" s="3">
-        <v>100</v>
-      </c>
-      <c r="E123" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E123" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
@@ -12603,13 +13076,17 @@
       <c r="B124" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>276</v>
+      <c r="C124" s="3">
+        <v>1</v>
       </c>
       <c r="D124" s="3">
-        <v>100</v>
-      </c>
-      <c r="E124" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E124" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
@@ -12673,13 +13150,17 @@
       <c r="B125" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C125" s="3" t="s">
-        <v>276</v>
+      <c r="C125" s="3">
+        <v>1</v>
       </c>
       <c r="D125" s="3">
-        <v>100</v>
-      </c>
-      <c r="E125" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E125" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
@@ -12743,13 +13224,17 @@
       <c r="B126" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="C126" s="3" t="s">
-        <v>276</v>
+      <c r="C126" s="3">
+        <v>1</v>
       </c>
       <c r="D126" s="3">
-        <v>100</v>
-      </c>
-      <c r="E126" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E126" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
@@ -12813,13 +13298,17 @@
       <c r="B127" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C127" s="3" t="s">
-        <v>276</v>
+      <c r="C127" s="3">
+        <v>1</v>
       </c>
       <c r="D127" s="3">
-        <v>100</v>
-      </c>
-      <c r="E127" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E127" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
@@ -12883,13 +13372,17 @@
       <c r="B128" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="C128" s="3" t="s">
-        <v>276</v>
+      <c r="C128" s="3">
+        <v>1</v>
       </c>
       <c r="D128" s="3">
-        <v>100</v>
-      </c>
-      <c r="E128" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E128" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F128" s="3"/>
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
@@ -12953,13 +13446,17 @@
       <c r="B129" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="C129" s="3" t="s">
-        <v>276</v>
+      <c r="C129" s="3">
+        <v>1</v>
       </c>
       <c r="D129" s="3">
-        <v>100</v>
-      </c>
-      <c r="E129" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E129" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
@@ -13023,13 +13520,17 @@
       <c r="B130" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="C130" s="3" t="s">
-        <v>276</v>
+      <c r="C130" s="3">
+        <v>1</v>
       </c>
       <c r="D130" s="3">
-        <v>100</v>
-      </c>
-      <c r="E130" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E130" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F130" s="3"/>
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
@@ -13093,13 +13594,17 @@
       <c r="B131" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="C131" s="3" t="s">
-        <v>276</v>
+      <c r="C131" s="3">
+        <v>1</v>
       </c>
       <c r="D131" s="3">
-        <v>100</v>
-      </c>
-      <c r="E131" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E131" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F131" s="3"/>
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
@@ -13163,13 +13668,17 @@
       <c r="B132" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="C132" s="3" t="s">
-        <v>276</v>
+      <c r="C132" s="3">
+        <v>1</v>
       </c>
       <c r="D132" s="3">
-        <v>100</v>
-      </c>
-      <c r="E132" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E132" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F132" s="3"/>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
@@ -13233,13 +13742,17 @@
       <c r="B133" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="C133" s="3" t="s">
-        <v>276</v>
+      <c r="C133" s="3">
+        <v>1</v>
       </c>
       <c r="D133" s="3">
-        <v>100</v>
-      </c>
-      <c r="E133" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E133" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F133" s="3"/>
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
@@ -13303,13 +13816,17 @@
       <c r="B134" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="C134" s="3" t="s">
-        <v>276</v>
+      <c r="C134" s="3">
+        <v>1</v>
       </c>
       <c r="D134" s="3">
-        <v>100</v>
-      </c>
-      <c r="E134" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E134" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F134" s="3"/>
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
@@ -13373,13 +13890,17 @@
       <c r="B135" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C135" s="3" t="s">
-        <v>276</v>
+      <c r="C135" s="3">
+        <v>1</v>
       </c>
       <c r="D135" s="3">
-        <v>100</v>
-      </c>
-      <c r="E135" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E135" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F135" s="3"/>
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
@@ -13443,13 +13964,17 @@
       <c r="B136" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="C136" s="3" t="s">
-        <v>276</v>
+      <c r="C136" s="3">
+        <v>1</v>
       </c>
       <c r="D136" s="3">
-        <v>100</v>
-      </c>
-      <c r="E136" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E136" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F136" s="3"/>
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
@@ -13513,13 +14038,17 @@
       <c r="B137" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C137" s="3" t="s">
-        <v>276</v>
+      <c r="C137" s="3">
+        <v>1</v>
       </c>
       <c r="D137" s="3">
-        <v>100</v>
-      </c>
-      <c r="E137" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E137" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F137" s="3"/>
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
@@ -13583,13 +14112,17 @@
       <c r="B138" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C138" s="3" t="s">
-        <v>276</v>
+      <c r="C138" s="3">
+        <v>1</v>
       </c>
       <c r="D138" s="3">
-        <v>100</v>
-      </c>
-      <c r="E138" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E138" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F138" s="3"/>
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
@@ -13653,13 +14186,17 @@
       <c r="B139" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C139" s="3" t="s">
-        <v>276</v>
+      <c r="C139" s="3">
+        <v>1</v>
       </c>
       <c r="D139" s="3">
-        <v>100</v>
-      </c>
-      <c r="E139" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E139" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F139" s="3"/>
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
@@ -13723,13 +14260,17 @@
       <c r="B140" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="C140" s="3" t="s">
-        <v>276</v>
+      <c r="C140" s="3">
+        <v>1</v>
       </c>
       <c r="D140" s="3">
-        <v>100</v>
-      </c>
-      <c r="E140" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E140" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F140" s="3"/>
       <c r="G140" s="3"/>
       <c r="H140" s="3"/>
@@ -13793,13 +14334,17 @@
       <c r="B141" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="C141" s="3" t="s">
-        <v>276</v>
+      <c r="C141" s="3">
+        <v>1</v>
       </c>
       <c r="D141" s="3">
-        <v>100</v>
-      </c>
-      <c r="E141" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E141" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F141" s="3"/>
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
@@ -13863,13 +14408,17 @@
       <c r="B142" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="C142" s="3" t="s">
-        <v>276</v>
+      <c r="C142" s="3">
+        <v>1</v>
       </c>
       <c r="D142" s="3">
-        <v>100</v>
-      </c>
-      <c r="E142" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E142" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F142" s="3"/>
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
@@ -13933,13 +14482,17 @@
       <c r="B143" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C143" s="3" t="s">
-        <v>276</v>
+      <c r="C143" s="3">
+        <v>1</v>
       </c>
       <c r="D143" s="3">
-        <v>100</v>
-      </c>
-      <c r="E143" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E143" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F143" s="3"/>
       <c r="G143" s="3"/>
       <c r="H143" s="3"/>
@@ -14003,13 +14556,17 @@
       <c r="B144" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="C144" s="3" t="s">
-        <v>276</v>
+      <c r="C144" s="3">
+        <v>1</v>
       </c>
       <c r="D144" s="3">
-        <v>100</v>
-      </c>
-      <c r="E144" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E144" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F144" s="3"/>
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
@@ -14073,13 +14630,17 @@
       <c r="B145" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="C145" s="3" t="s">
-        <v>276</v>
+      <c r="C145" s="3">
+        <v>1</v>
       </c>
       <c r="D145" s="3">
-        <v>100</v>
-      </c>
-      <c r="E145" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E145" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F145" s="3"/>
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
@@ -14143,13 +14704,17 @@
       <c r="B146" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="C146" s="3" t="s">
-        <v>276</v>
+      <c r="C146" s="3">
+        <v>1</v>
       </c>
       <c r="D146" s="3">
-        <v>100</v>
-      </c>
-      <c r="E146" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E146" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F146" s="3"/>
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
@@ -14213,13 +14778,17 @@
       <c r="B147" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C147" s="3" t="s">
-        <v>276</v>
+      <c r="C147" s="3">
+        <v>1</v>
       </c>
       <c r="D147" s="3">
-        <v>100</v>
-      </c>
-      <c r="E147" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E147" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F147" s="3"/>
       <c r="G147" s="3"/>
       <c r="H147" s="3"/>
@@ -14283,13 +14852,17 @@
       <c r="B148" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="C148" s="3" t="s">
-        <v>276</v>
+      <c r="C148" s="3">
+        <v>1</v>
       </c>
       <c r="D148" s="3">
-        <v>100</v>
-      </c>
-      <c r="E148" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E148" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F148" s="3"/>
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
@@ -14353,13 +14926,17 @@
       <c r="B149" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="C149" s="3" t="s">
-        <v>276</v>
+      <c r="C149" s="3">
+        <v>1</v>
       </c>
       <c r="D149" s="3">
-        <v>100</v>
-      </c>
-      <c r="E149" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E149" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F149" s="3"/>
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
@@ -14423,13 +15000,17 @@
       <c r="B150" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="C150" s="3" t="s">
-        <v>276</v>
+      <c r="C150" s="3">
+        <v>1</v>
       </c>
       <c r="D150" s="3">
-        <v>100</v>
-      </c>
-      <c r="E150" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E150" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F150" s="3"/>
       <c r="G150" s="3"/>
       <c r="H150" s="3"/>
@@ -14493,13 +15074,17 @@
       <c r="B151" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="C151" s="3" t="s">
-        <v>276</v>
+      <c r="C151" s="3">
+        <v>1</v>
       </c>
       <c r="D151" s="3">
-        <v>100</v>
-      </c>
-      <c r="E151" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E151" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F151" s="3"/>
       <c r="G151" s="3"/>
       <c r="H151" s="3"/>
@@ -14563,13 +15148,17 @@
       <c r="B152" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="C152" s="3" t="s">
-        <v>276</v>
+      <c r="C152" s="3">
+        <v>1</v>
       </c>
       <c r="D152" s="3">
-        <v>100</v>
-      </c>
-      <c r="E152" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E152" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F152" s="3"/>
       <c r="G152" s="3"/>
       <c r="H152" s="3"/>
@@ -14633,13 +15222,17 @@
       <c r="B153" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C153" s="3" t="s">
-        <v>276</v>
+      <c r="C153" s="3">
+        <v>1</v>
       </c>
       <c r="D153" s="3">
-        <v>100</v>
-      </c>
-      <c r="E153" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E153" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F153" s="3"/>
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
@@ -14703,13 +15296,17 @@
       <c r="B154" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="C154" s="3" t="s">
-        <v>276</v>
+      <c r="C154" s="3">
+        <v>1</v>
       </c>
       <c r="D154" s="3">
-        <v>100</v>
-      </c>
-      <c r="E154" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E154" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
@@ -14773,13 +15370,17 @@
       <c r="B155" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="C155" s="3" t="s">
-        <v>276</v>
+      <c r="C155" s="3">
+        <v>1</v>
       </c>
       <c r="D155" s="3">
-        <v>100</v>
-      </c>
-      <c r="E155" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E155" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F155" s="3"/>
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
@@ -14843,13 +15444,17 @@
       <c r="B156" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C156" s="3" t="s">
-        <v>276</v>
+      <c r="C156" s="3">
+        <v>1</v>
       </c>
       <c r="D156" s="3">
-        <v>100</v>
-      </c>
-      <c r="E156" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E156" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F156" s="3"/>
       <c r="G156" s="3"/>
       <c r="H156" s="3"/>
@@ -14913,13 +15518,17 @@
       <c r="B157" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="C157" s="3" t="s">
-        <v>276</v>
+      <c r="C157" s="3">
+        <v>1</v>
       </c>
       <c r="D157" s="3">
-        <v>100</v>
-      </c>
-      <c r="E157" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E157" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F157" s="3"/>
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
@@ -14983,13 +15592,17 @@
       <c r="B158" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="C158" s="3" t="s">
-        <v>276</v>
+      <c r="C158" s="3">
+        <v>1</v>
       </c>
       <c r="D158" s="3">
-        <v>100</v>
-      </c>
-      <c r="E158" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E158" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F158" s="3"/>
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
@@ -15053,13 +15666,17 @@
       <c r="B159" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="C159" s="3" t="s">
-        <v>276</v>
+      <c r="C159" s="3">
+        <v>1</v>
       </c>
       <c r="D159" s="3">
-        <v>100</v>
-      </c>
-      <c r="E159" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E159" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F159" s="3"/>
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
@@ -15123,13 +15740,17 @@
       <c r="B160" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="C160" s="3" t="s">
-        <v>276</v>
+      <c r="C160" s="3">
+        <v>1</v>
       </c>
       <c r="D160" s="3">
-        <v>100</v>
-      </c>
-      <c r="E160" s="3"/>
+        <f>Table5[[#This Row],[Column3]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="E160" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>3</v>
+      </c>
       <c r="F160" s="3"/>
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
@@ -15190,7 +15811,10 @@
       <c r="B161" s="14"/>
       <c r="C161" s="32"/>
       <c r="D161" s="32"/>
-      <c r="E161" s="32"/>
+      <c r="E161" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>0</v>
+      </c>
       <c r="F161" s="32"/>
       <c r="G161" s="32"/>
       <c r="H161" s="32"/>
@@ -15251,7 +15875,10 @@
       <c r="B162" s="14"/>
       <c r="C162" s="32"/>
       <c r="D162" s="32"/>
-      <c r="E162" s="32"/>
+      <c r="E162" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>0</v>
+      </c>
       <c r="F162" s="32"/>
       <c r="G162" s="32"/>
       <c r="H162" s="32"/>
@@ -15312,7 +15939,10 @@
       <c r="B163" s="14"/>
       <c r="C163" s="32"/>
       <c r="D163" s="32"/>
-      <c r="E163" s="32"/>
+      <c r="E163" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>0</v>
+      </c>
       <c r="F163" s="32"/>
       <c r="G163" s="32"/>
       <c r="H163" s="32"/>
@@ -15373,7 +16003,10 @@
       <c r="B164" s="14"/>
       <c r="C164" s="32"/>
       <c r="D164" s="32"/>
-      <c r="E164" s="32"/>
+      <c r="E164" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>0</v>
+      </c>
       <c r="F164" s="32"/>
       <c r="G164" s="32"/>
       <c r="H164" s="32"/>
@@ -15434,7 +16067,10 @@
       <c r="B165" s="14"/>
       <c r="C165" s="32"/>
       <c r="D165" s="32"/>
-      <c r="E165" s="32"/>
+      <c r="E165" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>0</v>
+      </c>
       <c r="F165" s="32"/>
       <c r="G165" s="32"/>
       <c r="H165" s="32"/>
@@ -15495,7 +16131,10 @@
       <c r="B166" s="14"/>
       <c r="C166" s="32"/>
       <c r="D166" s="32"/>
-      <c r="E166" s="32"/>
+      <c r="E166" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>0</v>
+      </c>
       <c r="F166" s="32"/>
       <c r="G166" s="32"/>
       <c r="H166" s="32"/>
@@ -15556,7 +16195,10 @@
       <c r="B167" s="14"/>
       <c r="C167" s="32"/>
       <c r="D167" s="32"/>
-      <c r="E167" s="32"/>
+      <c r="E167" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>0</v>
+      </c>
       <c r="F167" s="32"/>
       <c r="G167" s="32"/>
       <c r="H167" s="32"/>
@@ -15617,7 +16259,10 @@
       <c r="B168" s="14"/>
       <c r="C168" s="32"/>
       <c r="D168" s="32"/>
-      <c r="E168" s="32"/>
+      <c r="E168" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>0</v>
+      </c>
       <c r="F168" s="32"/>
       <c r="G168" s="32"/>
       <c r="H168" s="32"/>
@@ -15678,7 +16323,10 @@
       <c r="B169" s="14"/>
       <c r="C169" s="32"/>
       <c r="D169" s="32"/>
-      <c r="E169" s="32"/>
+      <c r="E169" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>0</v>
+      </c>
       <c r="F169" s="32"/>
       <c r="G169" s="32"/>
       <c r="H169" s="32"/>
@@ -15739,7 +16387,10 @@
       <c r="B170" s="14"/>
       <c r="C170" s="32"/>
       <c r="D170" s="32"/>
-      <c r="E170" s="32"/>
+      <c r="E170" s="3">
+        <f>Table5[[#This Row],[Column3]]+Table5[[#This Row],[Column4]]</f>
+        <v>0</v>
+      </c>
       <c r="F170" s="32"/>
       <c r="G170" s="32"/>
       <c r="H170" s="32"/>
@@ -15798,12 +16449,12 @@
     </row>
     <row r="171" spans="2:60" x14ac:dyDescent="0.25">
       <c r="B171" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="172" spans="2:60" x14ac:dyDescent="0.25">
       <c r="B172" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>